<commit_message>
iam committing my code.
</commit_message>
<xml_diff>
--- a/Resources/BRMSdata.xlsx
+++ b/Resources/BRMSdata.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vaishnavi.t\eclipse-workspace\BRMS2.0\Resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14265" windowHeight="5610" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14070" windowHeight="5610" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Department" sheetId="1" r:id="rId1"/>
@@ -21,8 +16,10 @@
     <sheet name="UOM" sheetId="8" r:id="rId7"/>
     <sheet name="Productdetails" sheetId="9" r:id="rId8"/>
     <sheet name="Strength" sheetId="6" r:id="rId9"/>
+    <sheet name="BPRproductdetails" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:L15"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="117">
   <si>
     <t>firstName</t>
   </si>
@@ -85,9 +82,6 @@
     <t>location1</t>
   </si>
   <si>
-    <t>QA-11</t>
-  </si>
-  <si>
     <t>Market</t>
   </si>
   <si>
@@ -181,48 +175,12 @@
     <t>20</t>
   </si>
   <si>
-    <t>Block-A</t>
-  </si>
-  <si>
-    <t>Injection Lyohilization</t>
-  </si>
-  <si>
-    <t>Injection Lyohilization11</t>
-  </si>
-  <si>
-    <t>China1</t>
-  </si>
-  <si>
-    <t>China</t>
-  </si>
-  <si>
-    <t>Strip packing2</t>
-  </si>
-  <si>
-    <t>Primary</t>
-  </si>
-  <si>
-    <t>10/30mg</t>
-  </si>
-  <si>
-    <t>10/30</t>
-  </si>
-  <si>
     <t>PK1</t>
   </si>
   <si>
     <t>PK</t>
   </si>
   <si>
-    <t>QC</t>
-  </si>
-  <si>
-    <t>Bottles Packing</t>
-  </si>
-  <si>
-    <t>Block-AB</t>
-  </si>
-  <si>
     <t>Europe</t>
   </si>
   <si>
@@ -250,22 +208,178 @@
     <t>1010001</t>
   </si>
   <si>
-    <t>Abilify</t>
-  </si>
-  <si>
-    <t>Common blend for Acetaminophen Suppositories Tablet 750 mg and 850 mg</t>
-  </si>
-  <si>
-    <t>650/750/850</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
-    <t>130.890</t>
-  </si>
-  <si>
-    <t>1010500</t>
+    <t>Germany1</t>
+  </si>
+  <si>
+    <t>Injection Liquid</t>
+  </si>
+  <si>
+    <t>Injection Liquid1</t>
+  </si>
+  <si>
+    <t>Sachets</t>
+  </si>
+  <si>
+    <t>Sachets1</t>
+  </si>
+  <si>
+    <t>Primary-Sachets1</t>
+  </si>
+  <si>
+    <t>Primary-Sachets</t>
+  </si>
+  <si>
+    <t>addpackstyle</t>
+  </si>
+  <si>
+    <t>Sachets2</t>
+  </si>
+  <si>
+    <t>10/250mg</t>
+  </si>
+  <si>
+    <t>250</t>
+  </si>
+  <si>
+    <t>prodname</t>
+  </si>
+  <si>
+    <t>prodcode</t>
+  </si>
+  <si>
+    <t>sfgcode</t>
+  </si>
+  <si>
+    <t>customerbatch</t>
+  </si>
+  <si>
+    <t>100's count</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Acyclovir</t>
+  </si>
+  <si>
+    <t>3003110</t>
+  </si>
+  <si>
+    <t>121.28</t>
+  </si>
+  <si>
+    <t>130.28</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Line-1</t>
+  </si>
+  <si>
+    <t>Line-11</t>
+  </si>
+  <si>
+    <t>Granulation11</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>location2</t>
+  </si>
+  <si>
+    <t>Line-2</t>
+  </si>
+  <si>
+    <t>Common bulk for Acetaminophen Suppositories Tablet 750 mg and 950 mg</t>
+  </si>
+  <si>
+    <t>170.890</t>
+  </si>
+  <si>
+    <t>2003001</t>
+  </si>
+  <si>
+    <t>156.890</t>
+  </si>
+  <si>
+    <t>1270.890</t>
+  </si>
+  <si>
+    <t>1570.890</t>
+  </si>
+  <si>
+    <t>Aripiprazole 250mg</t>
+  </si>
+  <si>
+    <t>159.890</t>
+  </si>
+  <si>
+    <t>MPRNo.</t>
+  </si>
+  <si>
+    <t>Common blend for Amoxicillin Suppositories Tablet 750 mg and 950 mg</t>
+  </si>
+  <si>
+    <t>2003001-02-00</t>
+  </si>
+  <si>
+    <t>Pellets/BlendMPRNo.</t>
+  </si>
+  <si>
+    <t>Common bulk for Amoxicillin Suppositories Tablet 750 mg and 950 mg</t>
+  </si>
+  <si>
+    <t>BMRMPRNo.</t>
+  </si>
+  <si>
+    <t>BPRMPRNo.</t>
+  </si>
+  <si>
+    <t>3001001</t>
+  </si>
+  <si>
+    <t>Amoxicillin</t>
+  </si>
+  <si>
+    <t>3002002</t>
+  </si>
+  <si>
+    <t>2003005</t>
+  </si>
+  <si>
+    <t>2003006</t>
+  </si>
+  <si>
+    <t>2003007</t>
+  </si>
+  <si>
+    <t>2003008</t>
+  </si>
+  <si>
+    <t>2003009</t>
+  </si>
+  <si>
+    <t>2003006-02-00</t>
+  </si>
+  <si>
+    <t>2003008-01-00</t>
+  </si>
+  <si>
+    <t>2003003-01-00</t>
+  </si>
+  <si>
+    <t>3002009</t>
+  </si>
+  <si>
+    <t>3002009-01-00</t>
   </si>
 </sst>
 </file>
@@ -619,6 +733,218 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="13.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="L2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="N2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="P2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="L3" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="N3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J4" t="s">
+        <v>53</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="L4" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="N4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
@@ -699,15 +1025,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -720,19 +1050,25 @@
       <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>83</v>
+      </c>
+      <c r="E2" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -746,7 +1082,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -756,18 +1092,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -781,7 +1117,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -792,18 +1128,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -814,10 +1150,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -825,34 +1161,41 @@
     <col min="2" max="2" width="10.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>55</v>
+      <c r="E1" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" t="s">
-        <v>55</v>
+        <v>64</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>63</v>
+      </c>
+      <c r="E2" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -866,7 +1209,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -877,30 +1220,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -911,10 +1254,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -923,135 +1266,335 @@
     <col min="4" max="4" width="10.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="M1" s="4" t="s">
+      <c r="E2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="N2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="F4" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J4" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="H2" t="s">
-        <v>66</v>
-      </c>
-      <c r="I2" s="3" t="s">
+      <c r="K4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" t="s">
         <v>76</v>
       </c>
-      <c r="J2" t="s">
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="J5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" t="s">
         <v>43</v>
       </c>
-      <c r="K2" t="s">
-        <v>44</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="L5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="J6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="L6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N6" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H3" t="s">
-        <v>66</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="J3" t="s">
+    </row>
+    <row r="7" spans="1:17" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="J7" t="s">
+        <v>42</v>
+      </c>
+      <c r="K7" t="s">
         <v>43</v>
       </c>
-      <c r="K3" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>43</v>
+      <c r="L7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N7" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1065,7 +1608,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1075,18 +1618,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
iam committing my code changes
</commit_message>
<xml_diff>
--- a/Resources/BRMSdata.xlsx
+++ b/Resources/BRMSdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14070" windowHeight="5610" firstSheet="6" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14070" windowHeight="5610" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Department" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="122">
   <si>
     <t>firstName</t>
   </si>
@@ -185,9 +185,6 @@
     <t>PK</t>
   </si>
   <si>
-    <t>Europe</t>
-  </si>
-  <si>
     <t>Capsule</t>
   </si>
   <si>
@@ -308,9 +305,6 @@
     <t>170.890</t>
   </si>
   <si>
-    <t>2003001</t>
-  </si>
-  <si>
     <t>156.890</t>
   </si>
   <si>
@@ -332,9 +326,6 @@
     <t>Common blend for Amoxicillin Suppositories Tablet 750 mg and 950 mg</t>
   </si>
   <si>
-    <t>2003001-02-00</t>
-  </si>
-  <si>
     <t>Pellets/BlendMPRNo.</t>
   </si>
   <si>
@@ -356,41 +347,65 @@
     <t>3002002</t>
   </si>
   <si>
-    <t>2003005</t>
-  </si>
-  <si>
-    <t>2003006</t>
-  </si>
-  <si>
-    <t>2003007</t>
-  </si>
-  <si>
-    <t>2003008</t>
-  </si>
-  <si>
-    <t>2003009</t>
-  </si>
-  <si>
     <t>2003003-01-00</t>
   </si>
   <si>
     <t>3002009</t>
   </si>
   <si>
-    <t>3002009-01-00</t>
-  </si>
-  <si>
-    <t>2003008-02-00</t>
-  </si>
-  <si>
-    <t>2003006-05-00</t>
+    <t>GM</t>
+  </si>
+  <si>
+    <t>2003011</t>
+  </si>
+  <si>
+    <t>BMR/2003012-01-00</t>
+  </si>
+  <si>
+    <t>BMR/2003012-02-01</t>
+  </si>
+  <si>
+    <t>2003021</t>
+  </si>
+  <si>
+    <t>2003022</t>
+  </si>
+  <si>
+    <t>2003023</t>
+  </si>
+  <si>
+    <t>2003024</t>
+  </si>
+  <si>
+    <t>BMR/2003021-02-00</t>
+  </si>
+  <si>
+    <t>BMR/2003021-03-00</t>
+  </si>
+  <si>
+    <t>BMR/2003023-01-00</t>
+  </si>
+  <si>
+    <t>BPR-8541225-01-00</t>
+  </si>
+  <si>
+    <t>BMR/2003021-07-00</t>
+  </si>
+  <si>
+    <t>BMR/2003023-02-00</t>
+  </si>
+  <si>
+    <t>BMR/2003021-06-01</t>
+  </si>
+  <si>
+    <t>BMR/2003021-06-02</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -410,6 +425,13 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -433,7 +455,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -444,6 +466,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -742,7 +765,7 @@
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -752,7 +775,8 @@
     <col min="6" max="6" width="10.625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -760,13 +784,13 @@
         <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>33</v>
@@ -793,33 +817,33 @@
         <v>36</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>39</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" t="s">
         <v>75</v>
-      </c>
-      <c r="B2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E2" t="s">
-        <v>76</v>
       </c>
       <c r="F2" t="s">
         <v>40</v>
@@ -831,45 +855,45 @@
         <v>41</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L2" t="s">
         <v>42</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N2" t="s">
         <v>43</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>114</v>
+      <c r="O2" t="s">
+        <v>117</v>
       </c>
       <c r="P2" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" t="s">
         <v>75</v>
-      </c>
-      <c r="B3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E3" t="s">
-        <v>76</v>
       </c>
       <c r="F3" t="s">
         <v>40</v>
@@ -881,19 +905,19 @@
         <v>41</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L3" t="s">
         <v>42</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N3" t="s">
         <v>43</v>
@@ -901,19 +925,19 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" t="s">
         <v>75</v>
-      </c>
-      <c r="B4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E4" t="s">
-        <v>76</v>
       </c>
       <c r="F4" t="s">
         <v>40</v>
@@ -925,19 +949,19 @@
         <v>41</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L4" t="s">
         <v>42</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N4" t="s">
         <v>43</v>
@@ -1055,24 +1079,24 @@
         <v>16</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" t="s">
         <v>84</v>
       </c>
-      <c r="C2" t="s">
-        <v>85</v>
-      </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1086,7 +1110,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1104,10 +1128,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1140,10 +1164,10 @@
     </row>
     <row r="2" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1182,24 +1206,24 @@
         <v>26</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>66</v>
-      </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1260,8 +1284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1270,9 +1294,7 @@
     <col min="4" max="4" width="10.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="18.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="47.25" x14ac:dyDescent="0.25">
@@ -1319,51 +1341,51 @@
         <v>36</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="P1" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="P1" s="4" t="s">
-        <v>100</v>
-      </c>
       <c r="Q1" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D2" t="s">
         <v>40</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
         <v>41</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J2" t="s">
-        <v>42</v>
+        <v>106</v>
       </c>
       <c r="K2" t="s">
         <v>43</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>47</v>
@@ -1371,52 +1393,50 @@
       <c r="N2" t="s">
         <v>42</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>99</v>
+      <c r="O2" t="s">
+        <v>121</v>
+      </c>
+      <c r="P2" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>91</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="B3" s="3"/>
       <c r="C3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" t="s">
         <v>50</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="F3" t="s">
         <v>41</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" t="s">
+        <v>106</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="J3" t="s">
-        <v>42</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="L3" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>44</v>
@@ -1424,43 +1444,52 @@
       <c r="N3" s="3" t="s">
         <v>42</v>
       </c>
+      <c r="O3" t="s">
+        <v>119</v>
+      </c>
+      <c r="P3" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>107</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="D4" t="s">
         <v>40</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F4" t="s">
         <v>41</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J4" t="s">
-        <v>42</v>
+        <v>106</v>
       </c>
       <c r="K4" t="s">
         <v>43</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>47</v>
@@ -1468,43 +1497,52 @@
       <c r="N4" t="s">
         <v>42</v>
       </c>
+      <c r="O4" t="s">
+        <v>116</v>
+      </c>
+      <c r="P4" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="5" spans="1:17" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
         <v>40</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F5" t="s">
         <v>41</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J5" t="s">
-        <v>42</v>
+        <v>106</v>
       </c>
       <c r="K5" t="s">
         <v>43</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>47</v>
@@ -1512,43 +1550,44 @@
       <c r="N5" t="s">
         <v>42</v>
       </c>
+      <c r="O5" s="6"/>
     </row>
     <row r="6" spans="1:17" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D6" t="s">
         <v>40</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F6" t="s">
         <v>41</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J6" t="s">
-        <v>42</v>
+        <v>106</v>
       </c>
       <c r="K6" t="s">
         <v>43</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>47</v>
@@ -1559,40 +1598,40 @@
     </row>
     <row r="7" spans="1:17" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D7" t="s">
         <v>40</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F7" t="s">
         <v>41</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J7" t="s">
-        <v>42</v>
+        <v>106</v>
       </c>
       <c r="K7" t="s">
         <v>43</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M7" s="3" t="s">
         <v>47</v>
@@ -1630,10 +1669,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committing my code to Git Repository by vaishnavi
</commit_message>
<xml_diff>
--- a/Resources/BRMSdata.xlsx
+++ b/Resources/BRMSdata.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vaishnavi.t\eclipse-workspace\BRMS2.0\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vaishnavi.T\eclipse-workspace\BRMS2.0\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14070" windowHeight="5610" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14070" windowHeight="5610" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Department" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="125">
   <si>
     <t>firstName</t>
   </si>
@@ -272,12 +272,6 @@
     <t>3003110</t>
   </si>
   <si>
-    <t>121.28</t>
-  </si>
-  <si>
-    <t>130.28</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -344,15 +338,6 @@
     <t>Amoxicillin</t>
   </si>
   <si>
-    <t>3002002</t>
-  </si>
-  <si>
-    <t>2003003-01-00</t>
-  </si>
-  <si>
-    <t>3002009</t>
-  </si>
-  <si>
     <t>GM</t>
   </si>
   <si>
@@ -386,19 +371,43 @@
     <t>BMR/2003023-01-00</t>
   </si>
   <si>
-    <t>BPR-8541225-01-00</t>
-  </si>
-  <si>
-    <t>BMR/2003021-07-00</t>
-  </si>
-  <si>
     <t>BMR/2003023-02-00</t>
   </si>
   <si>
-    <t>BMR/2003021-06-01</t>
-  </si>
-  <si>
-    <t>BMR/2003021-06-02</t>
+    <t>BMR/2003021-08-01</t>
+  </si>
+  <si>
+    <t>BMR/2003021-09-01</t>
+  </si>
+  <si>
+    <t>BMR/2003024-03-01</t>
+  </si>
+  <si>
+    <t>3002021</t>
+  </si>
+  <si>
+    <t>3002022</t>
+  </si>
+  <si>
+    <t>BMR/2003023-03-00</t>
+  </si>
+  <si>
+    <t>BPR/3002022-04-00</t>
+  </si>
+  <si>
+    <t>1611.28</t>
+  </si>
+  <si>
+    <t>1390.28</t>
+  </si>
+  <si>
+    <t>1211.28</t>
+  </si>
+  <si>
+    <t>1121.28</t>
+  </si>
+  <si>
+    <t>3002023</t>
   </si>
 </sst>
 </file>
@@ -754,7 +763,7 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -762,24 +771,24 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.58203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.08203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.58203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.08203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.25" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="18" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -823,13 +832,13 @@
         <v>39</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>74</v>
       </c>
@@ -837,7 +846,7 @@
         <v>77</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>78</v>
@@ -861,25 +870,25 @@
         <v>52</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>79</v>
+        <v>122</v>
       </c>
       <c r="L2" t="s">
         <v>42</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="N2" t="s">
         <v>43</v>
       </c>
       <c r="O2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="P2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -887,7 +896,7 @@
         <v>77</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>78</v>
@@ -911,27 +920,27 @@
         <v>52</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>80</v>
+        <v>121</v>
       </c>
       <c r="L3" t="s">
         <v>42</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="N3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>78</v>
@@ -955,15 +964,53 @@
         <v>52</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>79</v>
+        <v>120</v>
       </c>
       <c r="L4" t="s">
         <v>42</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="N4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="C5" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J5" t="s">
+        <v>52</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="L5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="N5" t="s">
         <v>43</v>
       </c>
     </row>
@@ -981,12 +1028,12 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -994,7 +1041,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1002,7 +1049,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1010,7 +1057,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1018,7 +1065,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1026,7 +1073,7 @@
         <v>8787878899</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1034,7 +1081,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1059,13 +1106,13 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -1079,24 +1126,24 @@
         <v>16</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1113,12 +1160,12 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="12.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
@@ -1126,12 +1173,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1148,13 +1195,13 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.08203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -1162,7 +1209,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="31" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>61</v>
       </c>
@@ -1184,15 +1231,15 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.08203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
@@ -1209,7 +1256,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>64</v>
       </c>
@@ -1240,13 +1287,13 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.58203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>27</v>
       </c>
@@ -1260,7 +1307,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -1284,20 +1331,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.58203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="45.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
@@ -1341,21 +1388,21 @@
         <v>36</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="P1" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="P1" s="4" t="s">
-        <v>97</v>
-      </c>
       <c r="Q1" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="47.25" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
         <v>75</v>
@@ -1376,10 +1423,10 @@
         <v>52</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="K2" t="s">
         <v>43</v>
@@ -1394,18 +1441,18 @@
         <v>42</v>
       </c>
       <c r="O2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="P2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="Q2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="47.25" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="62" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" t="s">
@@ -1430,7 +1477,7 @@
         <v>54</v>
       </c>
       <c r="J3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>55</v>
@@ -1445,21 +1492,21 @@
         <v>42</v>
       </c>
       <c r="O3" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="P3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="Q3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C4" t="s">
         <v>75</v>
@@ -1480,10 +1527,10 @@
         <v>52</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="K4" t="s">
         <v>43</v>
@@ -1498,21 +1545,21 @@
         <v>42</v>
       </c>
       <c r="O4" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="P4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="Q4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="47.25" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="62" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C5" t="s">
         <v>75</v>
@@ -1533,10 +1580,10 @@
         <v>52</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="K5" t="s">
         <v>43</v>
@@ -1552,12 +1599,12 @@
       </c>
       <c r="O5" s="6"/>
     </row>
-    <row r="6" spans="1:17" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C6" t="s">
         <v>75</v>
@@ -1578,10 +1625,10 @@
         <v>52</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J6" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="K6" t="s">
         <v>43</v>
@@ -1596,12 +1643,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="62" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C7" t="s">
         <v>75</v>
@@ -1622,10 +1669,10 @@
         <v>52</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J7" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="K7" t="s">
         <v>43</v>
@@ -1654,12 +1701,12 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="15.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
@@ -1667,7 +1714,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
i committing my code to my remote repository.
</commit_message>
<xml_diff>
--- a/Resources/BRMSdata.xlsx
+++ b/Resources/BRMSdata.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vaishnavi.T\eclipse-workspace\BRMS2.0\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14070" windowHeight="5610" firstSheet="4" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14070" windowHeight="5610" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Department" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="129">
   <si>
     <t>firstName</t>
   </si>
@@ -377,12 +377,6 @@
     <t>BMR/2003021-08-01</t>
   </si>
   <si>
-    <t>BMR/2003021-09-01</t>
-  </si>
-  <si>
-    <t>BMR/2003024-03-01</t>
-  </si>
-  <si>
     <t>3002021</t>
   </si>
   <si>
@@ -392,9 +386,6 @@
     <t>BMR/2003023-03-00</t>
   </si>
   <si>
-    <t>BPR/3002022-04-00</t>
-  </si>
-  <si>
     <t>1611.28</t>
   </si>
   <si>
@@ -408,12 +399,34 @@
   </si>
   <si>
     <t>3002023</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BPR/3002022-05-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BPR/3002022-05-00</t>
+  </si>
+  <si>
+    <t>ROW</t>
+  </si>
+  <si>
+    <t>BMR/2003021-13-00</t>
+  </si>
+  <si>
+    <t>BMR/2003022-04-00</t>
+  </si>
+  <si>
+    <t>BMR/2003023-04-00</t>
+  </si>
+  <si>
+    <t>BMR/2003024-04-00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -773,19 +786,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.58203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.08203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.58203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.08203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.58203125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.08203125"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.58203125"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="13.08203125"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="9.25"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="18.0"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="18.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
@@ -839,60 +852,60 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>74</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>77</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>75</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>40</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>41</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>52</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="L2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L2" t="s" s="0">
         <v>42</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="O2" t="s">
-        <v>119</v>
-      </c>
-      <c r="P2" t="s">
-        <v>118</v>
+      <c r="O2" t="s" s="0">
+        <v>122</v>
+      </c>
+      <c r="P2" t="s" s="0">
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>74</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>77</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -901,116 +914,119 @@
       <c r="D3" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>75</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>40</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>41</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>52</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="L3" t="s">
+        <v>118</v>
+      </c>
+      <c r="L3" t="s" s="0">
         <v>42</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" t="s" s="0">
         <v>43</v>
       </c>
+      <c r="O3" t="s" s="0">
+        <v>123</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>74</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>100</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>75</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>40</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>41</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>52</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="L4" t="s">
+        <v>117</v>
+      </c>
+      <c r="L4" t="s" s="0">
         <v>42</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" t="s" s="0">
         <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C5" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>75</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" t="s" s="0">
         <v>40</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>41</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" t="s" s="0">
         <v>52</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="L5" t="s">
+        <v>120</v>
+      </c>
+      <c r="L5" t="s" s="0">
         <v>42</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" t="s" s="0">
         <v>43</v>
       </c>
     </row>
@@ -1030,27 +1046,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.83203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1058,34 +1074,34 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="0">
         <v>8787878899</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>12</v>
       </c>
     </row>
@@ -1108,8 +1124,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.5"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -1130,19 +1146,19 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>82</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>81</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>82</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>80</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>85</v>
       </c>
     </row>
@@ -1162,7 +1178,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -1174,10 +1190,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>83</v>
       </c>
     </row>
@@ -1197,8 +1213,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.08203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.08203125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -1233,10 +1249,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.08203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.33203125"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.0"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.08203125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.83203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -1260,16 +1276,16 @@
       <c r="A2" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>63</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>62</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>67</v>
       </c>
     </row>
@@ -1289,8 +1305,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="14.58203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.58203125"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -1308,16 +1324,16 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>49</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>49</v>
       </c>
     </row>
@@ -1331,17 +1347,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.58203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.75"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.58203125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.83203125"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="9.75"/>
+    <col min="15" max="17" bestFit="true" customWidth="true" width="18.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="45.5" x14ac:dyDescent="0.35">
@@ -1404,31 +1420,31 @@
       <c r="B2" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>75</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>40</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>41</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>52</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>101</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>43</v>
       </c>
       <c r="L2" s="3" t="s">
@@ -1437,16 +1453,16 @@
       <c r="M2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="O2" t="s">
-        <v>115</v>
-      </c>
-      <c r="P2" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="O2" t="s" s="0">
+        <v>128</v>
+      </c>
+      <c r="P2" t="s" s="0">
+        <v>125</v>
+      </c>
+      <c r="Q2" t="s" s="0">
         <v>113</v>
       </c>
     </row>
@@ -1455,28 +1471,28 @@
         <v>86</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3" t="s" s="0">
+        <v>124</v>
+      </c>
+      <c r="D3" t="s" s="0">
         <v>50</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>41</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>52</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" t="s" s="0">
         <v>101</v>
       </c>
       <c r="K3" s="3" t="s">
@@ -1491,13 +1507,13 @@
       <c r="N3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" t="s" s="0">
         <v>112</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3" t="s" s="0">
         <v>110</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="Q3" t="s" s="0">
         <v>109</v>
       </c>
     </row>
@@ -1508,31 +1524,31 @@
       <c r="B4" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>75</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>40</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>41</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>52</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>101</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" t="s" s="0">
         <v>43</v>
       </c>
       <c r="L4" s="3" t="s">
@@ -1541,16 +1557,16 @@
       <c r="M4" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" t="s" s="0">
         <v>111</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P4" t="s" s="0">
         <v>104</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="Q4" t="s" s="0">
         <v>103</v>
       </c>
     </row>
@@ -1561,31 +1577,31 @@
       <c r="B5" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>75</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>40</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" t="s" s="0">
         <v>41</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>52</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" t="s" s="0">
         <v>101</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" t="s" s="0">
         <v>43</v>
       </c>
       <c r="L5" s="3" t="s">
@@ -1594,7 +1610,7 @@
       <c r="M5" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" t="s" s="0">
         <v>42</v>
       </c>
       <c r="O5" s="6"/>
@@ -1606,31 +1622,31 @@
       <c r="B6" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>75</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>40</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" t="s" s="0">
         <v>41</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>52</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" t="s" s="0">
         <v>101</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" t="s" s="0">
         <v>43</v>
       </c>
       <c r="L6" s="3" t="s">
@@ -1639,7 +1655,7 @@
       <c r="M6" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" t="s" s="0">
         <v>42</v>
       </c>
     </row>
@@ -1650,31 +1666,31 @@
       <c r="B7" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>75</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>40</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" t="s" s="0">
         <v>41</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" t="s" s="0">
         <v>52</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" t="s" s="0">
         <v>101</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" t="s" s="0">
         <v>43</v>
       </c>
       <c r="L7" s="3" t="s">
@@ -1683,7 +1699,7 @@
       <c r="M7" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" t="s" s="0">
         <v>42</v>
       </c>
     </row>
@@ -1703,7 +1719,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Iam committing my code to Remote repository.
</commit_message>
<xml_diff>
--- a/Resources/BRMSdata.xlsx
+++ b/Resources/BRMSdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vaishnavi.T\eclipse-workspace\BRMS2.0\Resources\"/>
     </mc:Choice>
@@ -25,7 +25,7 @@
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="130">
   <si>
     <t>firstName</t>
   </si>
@@ -338,9 +338,6 @@
     <t>Amoxicillin</t>
   </si>
   <si>
-    <t>GM</t>
-  </si>
-  <si>
     <t>2003011</t>
   </si>
   <si>
@@ -383,9 +380,6 @@
     <t>3002022</t>
   </si>
   <si>
-    <t>BMR/2003023-03-00</t>
-  </si>
-  <si>
     <t>1611.28</t>
   </si>
   <si>
@@ -401,9 +395,6 @@
     <t>3002023</t>
   </si>
   <si>
-    <t xml:space="preserve"> BPR/3002022-05-01</t>
-  </si>
-  <si>
     <t xml:space="preserve"> BPR/3002022-05-00</t>
   </si>
   <si>
@@ -413,21 +404,32 @@
     <t>BMR/2003021-13-00</t>
   </si>
   <si>
-    <t>BMR/2003022-04-00</t>
+    <t>Kg</t>
+  </si>
+  <si>
+    <t>BMR/2003021-17-00</t>
+  </si>
+  <si>
+    <t>BMR/2003024-04-00</t>
+  </si>
+  <si>
+    <t>FE250026</t>
   </si>
   <si>
     <t>BMR/2003023-04-00</t>
   </si>
   <si>
-    <t>BMR/2003024-04-00</t>
+    <t>BPR/3002021-01-00</t>
+  </si>
+  <si>
+    <t>BPR/4808303-01-00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -455,6 +457,11 @@
       <name val="Times New Roman"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF222222"/>
+      <name val="Source Sans Pro"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -477,7 +484,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -489,6 +496,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -776,7 +786,7 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -784,24 +794,24 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.58203125"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.08203125"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.58203125"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="13.08203125"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="9.25"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="18.0"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="18.33203125"/>
+    <col min="1" max="1" width="9.58203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.08203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.58203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.08203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -851,61 +861,61 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2" t="s" s="0">
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
         <v>74</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>77</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>75</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>40</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>41</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="J2" t="s" s="0">
+      <c r="J2" t="s">
         <v>52</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="L2" t="s" s="0">
+        <v>117</v>
+      </c>
+      <c r="L2" t="s">
         <v>42</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="N2" t="s" s="0">
+      <c r="N2" t="s">
         <v>43</v>
       </c>
-      <c r="O2" t="s" s="0">
-        <v>122</v>
-      </c>
-      <c r="P2" t="s" s="0">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A3" t="s" s="0">
+      <c r="O2" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="P2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" t="s">
         <v>74</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>77</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -914,121 +924,127 @@
       <c r="D3" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>75</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="F3" t="s">
         <v>40</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H3" t="s" s="0">
+      <c r="H3" t="s">
         <v>41</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="J3" t="s" s="0">
+      <c r="J3" t="s">
         <v>52</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="L3" t="s" s="0">
+        <v>116</v>
+      </c>
+      <c r="L3" t="s">
         <v>42</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="N3" t="s" s="0">
+      <c r="N3" t="s">
         <v>43</v>
       </c>
-      <c r="O3" t="s" s="0">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A4" t="s" s="0">
+      <c r="O3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" t="s">
         <v>74</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>100</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>75</v>
       </c>
-      <c r="F4" t="s" s="0">
+      <c r="F4" t="s">
         <v>40</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H4" t="s" s="0">
+      <c r="H4" t="s">
         <v>41</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="J4" t="s" s="0">
+      <c r="J4" t="s">
         <v>52</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="L4" t="s" s="0">
+        <v>115</v>
+      </c>
+      <c r="L4" t="s">
         <v>42</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="N4" t="s" s="0">
+      <c r="N4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="O4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="C5" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="E5" t="s">
         <v>75</v>
       </c>
-      <c r="F5" t="s" s="0">
+      <c r="F5" t="s">
         <v>40</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H5" t="s" s="0">
+      <c r="H5" t="s">
         <v>41</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="J5" t="s" s="0">
+      <c r="J5" t="s">
         <v>52</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="L5" t="s" s="0">
+        <v>118</v>
+      </c>
+      <c r="L5" t="s">
         <v>42</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="N5" t="s" s="0">
+      <c r="N5" t="s">
         <v>43</v>
       </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="O8" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1044,64 +1060,64 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.83203125"/>
+    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s" s="0">
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s" s="0">
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s" s="0">
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s" s="0">
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s" s="0">
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="0">
+      <c r="B5">
         <v>8787878899</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s" s="0">
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s" s="0">
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s" s="0">
+      <c r="B7" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1122,13 +1138,13 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.5"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.5"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -1145,20 +1161,20 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s" s="0">
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
         <v>82</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>81</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>82</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>80</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1176,12 +1192,12 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.25"/>
+    <col min="2" max="2" width="12.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
@@ -1189,11 +1205,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s" s="0">
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
         <v>59</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1211,13 +1227,13 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.08203125"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="13.5"/>
+    <col min="1" max="1" width="11.08203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -1225,7 +1241,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="31">
       <c r="A2" s="5" t="s">
         <v>61</v>
       </c>
@@ -1247,15 +1263,15 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.33203125"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.0"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.08203125"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.83203125"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.08203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
@@ -1272,20 +1288,20 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="31">
       <c r="A2" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>63</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>62</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1303,13 +1319,13 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.58203125"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.0"/>
+    <col min="3" max="3" width="14.58203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>27</v>
       </c>
@@ -1323,17 +1339,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s" s="0">
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
         <v>48</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>48</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>49</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1345,22 +1361,22 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="23.75"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.58203125"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.83203125"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="9.75"/>
-    <col min="15" max="17" bestFit="true" customWidth="true" width="18.33203125"/>
+    <col min="1" max="1" width="23.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.58203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="45.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="45.5">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
@@ -1413,38 +1429,38 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" ht="46.5">
       <c r="A2" s="5" t="s">
         <v>94</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C2" t="s" s="0">
+        <v>104</v>
+      </c>
+      <c r="C2" t="s">
         <v>75</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>40</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>41</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>52</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="J2" t="s" s="0">
-        <v>101</v>
-      </c>
-      <c r="K2" t="s" s="0">
+      <c r="J2" t="s">
+        <v>123</v>
+      </c>
+      <c r="K2" t="s">
         <v>43</v>
       </c>
       <c r="L2" s="3" t="s">
@@ -1453,47 +1469,50 @@
       <c r="M2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="N2" t="s" s="0">
+      <c r="N2" t="s">
         <v>42</v>
       </c>
-      <c r="O2" t="s" s="0">
-        <v>128</v>
-      </c>
-      <c r="P2" t="s" s="0">
-        <v>125</v>
-      </c>
-      <c r="Q2" t="s" s="0">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="62" x14ac:dyDescent="0.35">
+      <c r="O2" t="s">
+        <v>122</v>
+      </c>
+      <c r="P2" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>122</v>
+      </c>
+      <c r="R2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="62">
       <c r="A3" s="5" t="s">
         <v>86</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" t="s" s="0">
-        <v>124</v>
-      </c>
-      <c r="D3" t="s" s="0">
+      <c r="C3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3" t="s">
         <v>50</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="F3" t="s">
         <v>41</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H3" t="s" s="0">
+      <c r="H3" t="s">
         <v>52</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="J3" t="s" s="0">
-        <v>101</v>
+      <c r="J3" t="s">
+        <v>123</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>55</v>
@@ -1507,48 +1526,48 @@
       <c r="N3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="O3" t="s" s="0">
-        <v>112</v>
-      </c>
-      <c r="P3" t="s" s="0">
-        <v>110</v>
-      </c>
-      <c r="Q3" t="s" s="0">
+      <c r="O3" t="s">
+        <v>111</v>
+      </c>
+      <c r="P3" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" s="5" t="s">
         <v>91</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C4" t="s" s="0">
+        <v>101</v>
+      </c>
+      <c r="C4" t="s">
         <v>75</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>40</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F4" t="s" s="0">
+      <c r="F4" t="s">
         <v>41</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="H4" t="s" s="0">
+      <c r="H4" t="s">
         <v>52</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="J4" t="s" s="0">
-        <v>101</v>
-      </c>
-      <c r="K4" t="s" s="0">
+      <c r="J4" t="s">
+        <v>123</v>
+      </c>
+      <c r="K4" t="s">
         <v>43</v>
       </c>
       <c r="L4" s="3" t="s">
@@ -1557,51 +1576,54 @@
       <c r="M4" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="N4" t="s" s="0">
+      <c r="N4" t="s">
         <v>42</v>
       </c>
-      <c r="O4" t="s" s="0">
-        <v>111</v>
-      </c>
-      <c r="P4" t="s" s="0">
-        <v>104</v>
-      </c>
-      <c r="Q4" t="s" s="0">
+      <c r="O4" t="s">
+        <v>110</v>
+      </c>
+      <c r="P4" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" ht="62" x14ac:dyDescent="0.35">
+      <c r="Q4" t="s">
+        <v>102</v>
+      </c>
+      <c r="R4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="62">
       <c r="A5" s="5" t="s">
         <v>86</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C5" t="s" s="0">
+        <v>105</v>
+      </c>
+      <c r="C5" t="s">
         <v>75</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>40</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F5" t="s" s="0">
+      <c r="F5" t="s">
         <v>41</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="H5" t="s" s="0">
+      <c r="H5" t="s">
         <v>52</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="J5" t="s" s="0">
-        <v>101</v>
-      </c>
-      <c r="K5" t="s" s="0">
+      <c r="J5" t="s">
+        <v>123</v>
+      </c>
+      <c r="K5" t="s">
         <v>43</v>
       </c>
       <c r="L5" s="3" t="s">
@@ -1610,43 +1632,46 @@
       <c r="M5" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="N5" t="s" s="0">
+      <c r="N5" t="s">
         <v>42</v>
       </c>
       <c r="O5" s="6"/>
-    </row>
-    <row r="6" spans="1:17" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="Q5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="46.5">
       <c r="A6" s="5" t="s">
         <v>96</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C6" t="s" s="0">
+        <v>106</v>
+      </c>
+      <c r="C6" t="s">
         <v>75</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="D6" t="s">
         <v>40</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F6" t="s" s="0">
+      <c r="F6" t="s">
         <v>41</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="H6" t="s" s="0">
+      <c r="H6" t="s">
         <v>52</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="J6" t="s" s="0">
-        <v>101</v>
-      </c>
-      <c r="K6" t="s" s="0">
+      <c r="J6" t="s">
+        <v>123</v>
+      </c>
+      <c r="K6" t="s">
         <v>43</v>
       </c>
       <c r="L6" s="3" t="s">
@@ -1655,42 +1680,42 @@
       <c r="M6" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="N6" t="s" s="0">
+      <c r="N6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="62" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" ht="62">
       <c r="A7" s="5" t="s">
         <v>86</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C7" t="s" s="0">
+        <v>107</v>
+      </c>
+      <c r="C7" t="s">
         <v>75</v>
       </c>
-      <c r="D7" t="s" s="0">
+      <c r="D7" t="s">
         <v>40</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F7" t="s" s="0">
+      <c r="F7" t="s">
         <v>41</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="H7" t="s" s="0">
+      <c r="H7" t="s">
         <v>52</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="J7" t="s" s="0">
-        <v>101</v>
-      </c>
-      <c r="K7" t="s" s="0">
+      <c r="J7" t="s">
+        <v>123</v>
+      </c>
+      <c r="K7" t="s">
         <v>43</v>
       </c>
       <c r="L7" s="3" t="s">
@@ -1699,7 +1724,7 @@
       <c r="M7" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="N7" t="s" s="0">
+      <c r="N7" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1717,12 +1742,12 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.25"/>
+    <col min="2" max="2" width="15.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
@@ -1730,7 +1755,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
I am commiting the changes to remote repository
</commit_message>
<xml_diff>
--- a/Resources/BRMSdata.xlsx
+++ b/Resources/BRMSdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vaishnavi.T\eclipse-workspace\BRMS2.0\Resources\"/>
     </mc:Choice>
@@ -25,7 +25,7 @@
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="130">
   <si>
     <t>firstName</t>
   </si>
@@ -188,9 +188,6 @@
     <t>Capsule</t>
   </si>
   <si>
-    <t>10/20</t>
-  </si>
-  <si>
     <t>years</t>
   </si>
   <si>
@@ -203,12 +200,6 @@
     <t>Re-Initiated</t>
   </si>
   <si>
-    <t>1010000</t>
-  </si>
-  <si>
-    <t>1010001</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
@@ -257,179 +248,189 @@
     <t>customerbatch</t>
   </si>
   <si>
-    <t>100's count</t>
-  </si>
-  <si>
     <t>USA</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>Acyclovir</t>
-  </si>
-  <si>
     <t>3003110</t>
   </si>
   <si>
+    <t>Line-1</t>
+  </si>
+  <si>
+    <t>Line-11</t>
+  </si>
+  <si>
+    <t>Granulation11</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>location2</t>
+  </si>
+  <si>
+    <t>Line-2</t>
+  </si>
+  <si>
+    <t>MPRNo.</t>
+  </si>
+  <si>
+    <t>Pellets/BlendMPRNo.</t>
+  </si>
+  <si>
+    <t>BMRMPRNo.</t>
+  </si>
+  <si>
+    <t>BPRMPRNo.</t>
+  </si>
+  <si>
+    <t>ROW</t>
+  </si>
+  <si>
+    <t>Kg</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>Mg</t>
+  </si>
+  <si>
+    <t>759.890</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>ACY-T-004-00</t>
+  </si>
+  <si>
+    <t>No's</t>
+  </si>
+  <si>
+    <t>100' Count</t>
+  </si>
+  <si>
+    <t>200's Count</t>
+  </si>
+  <si>
+    <t>Atenolol</t>
+  </si>
+  <si>
+    <t>Telmisartan</t>
+  </si>
+  <si>
+    <t>BMR/2003012-02-00</t>
+  </si>
+  <si>
+    <t>Metformin Tablet 100 mg and 400 mg</t>
+  </si>
+  <si>
+    <t>BPR/7584985-02-04</t>
+  </si>
+  <si>
+    <t>BMR/2005300-03-00</t>
+  </si>
+  <si>
+    <t>120011.28</t>
+  </si>
+  <si>
+    <t>130190.28</t>
+  </si>
+  <si>
+    <t>161011.28</t>
+  </si>
+  <si>
+    <t>1120221.28</t>
+  </si>
+  <si>
     <t>No</t>
   </si>
   <si>
-    <t>Line-1</t>
-  </si>
-  <si>
-    <t>Line-11</t>
-  </si>
-  <si>
-    <t>Granulation11</t>
-  </si>
-  <si>
-    <t>Australia</t>
-  </si>
-  <si>
-    <t>location2</t>
-  </si>
-  <si>
-    <t>Line-2</t>
-  </si>
-  <si>
-    <t>Common bulk for Acetaminophen Suppositories Tablet 750 mg and 950 mg</t>
-  </si>
-  <si>
-    <t>170.890</t>
-  </si>
-  <si>
-    <t>156.890</t>
-  </si>
-  <si>
-    <t>1270.890</t>
-  </si>
-  <si>
-    <t>1570.890</t>
-  </si>
-  <si>
-    <t>Aripiprazole 250mg</t>
-  </si>
-  <si>
-    <t>159.890</t>
-  </si>
-  <si>
-    <t>MPRNo.</t>
-  </si>
-  <si>
-    <t>Common blend for Amoxicillin Suppositories Tablet 750 mg and 950 mg</t>
-  </si>
-  <si>
-    <t>Pellets/BlendMPRNo.</t>
-  </si>
-  <si>
-    <t>Common bulk for Amoxicillin Suppositories Tablet 750 mg and 950 mg</t>
-  </si>
-  <si>
-    <t>BMRMPRNo.</t>
-  </si>
-  <si>
-    <t>BPRMPRNo.</t>
-  </si>
-  <si>
-    <t>3001001</t>
-  </si>
-  <si>
-    <t>Amoxicillin</t>
-  </si>
-  <si>
-    <t>2003011</t>
-  </si>
-  <si>
-    <t>BMR/2003012-01-00</t>
-  </si>
-  <si>
-    <t>BMR/2003012-02-01</t>
-  </si>
-  <si>
-    <t>2003021</t>
-  </si>
-  <si>
-    <t>2003022</t>
-  </si>
-  <si>
-    <t>2003023</t>
-  </si>
-  <si>
-    <t>2003024</t>
-  </si>
-  <si>
-    <t>BMR/2003021-02-00</t>
-  </si>
-  <si>
-    <t>BMR/2003021-03-00</t>
-  </si>
-  <si>
-    <t>BMR/2003023-01-00</t>
-  </si>
-  <si>
-    <t>BMR/2003023-02-00</t>
-  </si>
-  <si>
-    <t>BMR/2003021-08-01</t>
-  </si>
-  <si>
-    <t>3002021</t>
-  </si>
-  <si>
-    <t>3002022</t>
-  </si>
-  <si>
-    <t>1611.28</t>
-  </si>
-  <si>
-    <t>1390.28</t>
-  </si>
-  <si>
-    <t>1211.28</t>
-  </si>
-  <si>
-    <t>1121.28</t>
-  </si>
-  <si>
-    <t>3002023</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> BPR/3002022-05-00</t>
-  </si>
-  <si>
-    <t>ROW</t>
-  </si>
-  <si>
-    <t>BMR/2003021-13-00</t>
-  </si>
-  <si>
-    <t>Kg</t>
-  </si>
-  <si>
-    <t>BMR/2003021-17-00</t>
-  </si>
-  <si>
-    <t>BMR/2003024-04-00</t>
-  </si>
-  <si>
-    <t>FE250026</t>
-  </si>
-  <si>
-    <t>BMR/2003023-04-00</t>
-  </si>
-  <si>
-    <t>BPR/3002021-01-00</t>
-  </si>
-  <si>
-    <t>BPR/4808303-01-00</t>
+    <t>3005004</t>
+  </si>
+  <si>
+    <t>200' Count</t>
+  </si>
+  <si>
+    <t>BPR/3005004-01-00</t>
+  </si>
+  <si>
+    <t>Ibuprofen Tablet 100 mg and 400 mg</t>
+  </si>
+  <si>
+    <t>Common bulk for Ibuprofen  Tablet 100 mg and 400 mg</t>
+  </si>
+  <si>
+    <t>2004001</t>
+  </si>
+  <si>
+    <t>2004002</t>
+  </si>
+  <si>
+    <t>2004003</t>
+  </si>
+  <si>
+    <t>2004004</t>
+  </si>
+  <si>
+    <t>2004005</t>
+  </si>
+  <si>
+    <t>1010120</t>
+  </si>
+  <si>
+    <t>1010121</t>
+  </si>
+  <si>
+    <t>1010122</t>
+  </si>
+  <si>
+    <t>1010123</t>
+  </si>
+  <si>
+    <t>1010124</t>
+  </si>
+  <si>
+    <t>1010125</t>
+  </si>
+  <si>
+    <t>Aripiprazole 400mg</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>BMR/2004001-01-00</t>
+  </si>
+  <si>
+    <t>2570.890</t>
+  </si>
+  <si>
+    <t>8176.890</t>
+  </si>
+  <si>
+    <t>9270.890</t>
+  </si>
+  <si>
+    <t>9570.890</t>
+  </si>
+  <si>
+    <t>8900.28</t>
+  </si>
+  <si>
+    <t>BMR/2004002-01-00</t>
+  </si>
+  <si>
+    <t>FE255037</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+  <numFmts count="0"/>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -456,11 +457,6 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF222222"/>
-      <name val="Source Sans Pro"/>
     </font>
   </fonts>
   <fills count="2">
@@ -496,9 +492,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -786,7 +780,7 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -796,33 +790,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.58203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.08203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.58203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.08203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.25"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.08203125"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.75"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.58203125"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="10.25"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="13.08203125"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="9.25"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="18.0"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="18.33203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>33</v>
@@ -849,202 +845,192 @@
         <v>36</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>39</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2" t="s" s="0">
+        <v>105</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>93</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="L2" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="N2" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="O2" t="s" s="0">
+        <v>106</v>
+      </c>
+      <c r="P2" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="P1" s="2" t="s">
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="L3" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="N3" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4" t="s" s="0">
+        <v>91</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>93</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L4" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="N4" t="s" s="0">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="L5" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="N5" t="s" s="0">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="M8" s="3"/>
+      <c r="O8" s="6" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J2" t="s">
-        <v>52</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="L2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="N2" t="s">
-        <v>43</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="P2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="A3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="J3" t="s">
-        <v>52</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="L3" t="s">
-        <v>42</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="N3" t="s">
-        <v>43</v>
-      </c>
-      <c r="O3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J4" t="s">
-        <v>52</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="L4" t="s">
-        <v>42</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="N4" t="s">
-        <v>43</v>
-      </c>
-      <c r="O4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="C5" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H5" t="s">
-        <v>41</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J5" t="s">
-        <v>52</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="L5" t="s">
-        <v>42</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="N5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="O8" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1060,64 +1046,64 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.83203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s" s="0">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="0">
         <v>8787878899</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>12</v>
       </c>
     </row>
@@ -1138,13 +1124,13 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.5"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -1158,24 +1144,24 @@
         <v>16</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E2" t="s">
-        <v>85</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1192,12 +1178,12 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
@@ -1205,12 +1191,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" t="s">
-        <v>83</v>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1227,13 +1213,13 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.08203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.08203125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -1241,12 +1227,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="31">
+    <row r="2" spans="1:2" ht="31" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1263,15 +1249,15 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.08203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.33203125"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.0"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.08203125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.83203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
@@ -1285,24 +1271,24 @@
         <v>26</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="31">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="E2" t="s" s="0">
         <v>64</v>
-      </c>
-      <c r="B2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E2" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1319,13 +1305,13 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="14.58203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.58203125"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>27</v>
       </c>
@@ -1339,17 +1325,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>49</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>49</v>
       </c>
     </row>
@@ -1363,20 +1349,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.58203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.75"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.58203125"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.83203125"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="9.75"/>
+    <col min="15" max="17" bestFit="true" customWidth="true" width="18.33203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="45.5">
+    <row r="1" spans="1:18" ht="45.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
@@ -1420,105 +1406,102 @@
         <v>36</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" ht="46.5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="31" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="D2" t="s" s="0">
         <v>40</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" t="s">
-        <v>41</v>
+        <v>53</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>86</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H2" t="s">
-        <v>52</v>
+        <v>55</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>51</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="J2" t="s">
         <v>123</v>
       </c>
-      <c r="K2" t="s">
+      <c r="J2" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="K2" t="s" s="0">
         <v>43</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>56</v>
+        <v>114</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" t="s" s="0">
+        <v>128</v>
+      </c>
+      <c r="P2" t="s" s="0">
         <v>122</v>
       </c>
-      <c r="P2" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>122</v>
-      </c>
-      <c r="R2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="62">
+      <c r="Q2" t="s" s="0">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="31" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" t="s" s="0">
         <v>86</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" t="s">
-        <v>121</v>
-      </c>
-      <c r="D3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="G3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" t="s" s="0">
         <v>51</v>
       </c>
-      <c r="F3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" t="s">
-        <v>52</v>
-      </c>
       <c r="I3" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="J3" t="s">
-        <v>123</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>57</v>
+      <c r="L3" s="7" t="s">
+        <v>115</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>44</v>
@@ -1526,205 +1509,183 @@
       <c r="N3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="O3" t="s">
-        <v>111</v>
-      </c>
-      <c r="P3" t="s">
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="Q3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
-      <c r="A4" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C4" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="D4" t="s" s="0">
         <v>40</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F4" t="s">
-        <v>41</v>
+        <v>53</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>86</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H4" t="s">
-        <v>52</v>
+        <v>55</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>51</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="J4" t="s">
-        <v>123</v>
-      </c>
-      <c r="K4" t="s">
+        <v>87</v>
+      </c>
+      <c r="J4" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="K4" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="L4" s="3" t="s">
-        <v>56</v>
+      <c r="L4" s="7" t="s">
+        <v>116</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="O4" t="s">
-        <v>110</v>
-      </c>
-      <c r="P4" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>102</v>
-      </c>
-      <c r="R4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="62">
+      <c r="R4" t="s" s="0">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="31" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" t="s" s="0">
         <v>86</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F5" t="s">
-        <v>41</v>
-      </c>
       <c r="G5" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H5" t="s">
-        <v>52</v>
+        <v>55</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>51</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="J5" t="s">
-        <v>123</v>
-      </c>
-      <c r="K5" t="s">
+        <v>124</v>
+      </c>
+      <c r="J5" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="K5" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="L5" s="3" t="s">
-        <v>56</v>
+      <c r="L5" s="7" t="s">
+        <v>117</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="O5" s="6"/>
-      <c r="Q5" t="s">
+    </row>
+    <row r="6" spans="1:18" ht="31" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" ht="46.5">
-      <c r="A6" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H6" t="s">
-        <v>52</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="J6" t="s">
-        <v>123</v>
-      </c>
-      <c r="K6" t="s">
+      <c r="J6" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="K6" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="L6" s="3" t="s">
-        <v>56</v>
+      <c r="L6" s="7" t="s">
+        <v>118</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" t="s" s="0">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="62">
+    <row r="7" spans="1:18" ht="31" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" t="s" s="0">
         <v>86</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F7" t="s">
-        <v>41</v>
-      </c>
       <c r="G7" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H7" t="s">
-        <v>52</v>
+        <v>55</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>51</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="J7" t="s">
-        <v>123</v>
-      </c>
-      <c r="K7" t="s">
+        <v>126</v>
+      </c>
+      <c r="J7" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="K7" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="L7" s="3" t="s">
-        <v>56</v>
+      <c r="L7" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="M7" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" t="s" s="0">
         <v>42</v>
       </c>
     </row>
@@ -1742,12 +1703,12 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
@@ -1755,12 +1716,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>